<commit_message>
added talks LIDS conference
</commit_message>
<xml_diff>
--- a/data/seminars.xlsx
+++ b/data/seminars.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="465">
   <si>
     <t>date</t>
   </si>
@@ -1394,10 +1394,28 @@
     <t>Canada</t>
   </si>
   <si>
-    <t>Contributed session</t>
-  </si>
-  <si>
     <t>Estimands and Safety in Oncology Clinical Trials</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Title Applying the estimands framework to time-to-event oncology studies: What happens when you cannot follow past an intercurrent event?</t>
+  </si>
+  <si>
+    <t>Invited talks</t>
+  </si>
+  <si>
+    <t>Liwei Wang</t>
+  </si>
+  <si>
+    <t>GenMab</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Title Logic respecting efficacy measures in the presence of prognostic or predictive biomarker subgroups</t>
+  </si>
+  <si>
+    <t>AbbVie</t>
+  </si>
+  <si>
+    <t>Estimands and treatment switching</t>
   </si>
 </sst>
 </file>
@@ -1788,11 +1806,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P123"/>
+  <dimension ref="A1:P125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N122" sqref="N122"/>
+      <selection pane="bottomLeft" activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4782,7 +4800,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="str">
         <f>"31.05.2023"</f>
         <v>31.05.2023</v>
@@ -4803,7 +4821,7 @@
         <v>338</v>
       </c>
       <c r="G115" s="8" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="K115" s="8">
         <v>1</v>
@@ -4814,65 +4832,76 @@
       <c r="M115" s="8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N115" s="9" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="8" t="str">
+        <f t="shared" ref="A116:A117" si="0">"31.05.2023"</f>
+        <v>31.05.2023</v>
+      </c>
+      <c r="C116" s="10"/>
+      <c r="K116" s="8">
+        <v>2</v>
+      </c>
+      <c r="L116" s="8" t="s">
+        <v>460</v>
+      </c>
+      <c r="M116" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="N116" s="9" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A117" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>31.05.2023</v>
+      </c>
+      <c r="C117" s="10"/>
+      <c r="K117" s="8">
+        <v>3</v>
+      </c>
+      <c r="L117" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="M117" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="N117" s="9" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A118" s="8" t="str">
         <f>"11.06.2023"</f>
         <v>11.06.2023</v>
       </c>
-      <c r="B116" s="9" t="s">
+      <c r="B118" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="C116" s="8" t="s">
+      <c r="C118" s="8" t="s">
         <v>438</v>
       </c>
-      <c r="D116" s="8" t="s">
+      <c r="D118" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E116" s="8" t="s">
+      <c r="E118" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F116" s="8" t="s">
+      <c r="F118" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="G116" s="8" t="s">
+      <c r="G118" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="K116" s="8">
-        <v>1</v>
-      </c>
-      <c r="L116" s="8" t="s">
+      <c r="K118" s="8">
+        <v>1</v>
+      </c>
+      <c r="L118" s="8" t="s">
         <v>440</v>
-      </c>
-      <c r="M116" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A117" s="8" t="str">
-        <f t="shared" ref="A117:A121" si="0">"11.06.2023"</f>
-        <v>11.06.2023</v>
-      </c>
-      <c r="K117" s="8">
-        <v>2</v>
-      </c>
-      <c r="L117" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="M117" s="8" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A118" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>11.06.2023</v>
-      </c>
-      <c r="K118" s="8">
-        <v>3</v>
-      </c>
-      <c r="L118" s="8" t="s">
-        <v>445</v>
       </c>
       <c r="M118" s="8" t="s">
         <v>52</v>
@@ -4880,115 +4909,145 @@
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A119:A123" si="1">"11.06.2023"</f>
         <v>11.06.2023</v>
       </c>
       <c r="K119" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L119" s="8" t="s">
-        <v>386</v>
+        <v>173</v>
       </c>
       <c r="M119" s="8" t="s">
-        <v>387</v>
+        <v>441</v>
       </c>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.06.2023</v>
       </c>
       <c r="K120" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L120" s="8" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="M120" s="8" t="s">
-        <v>443</v>
+        <v>52</v>
       </c>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.06.2023</v>
       </c>
       <c r="K121" s="8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L121" s="8" t="s">
-        <v>294</v>
+        <v>386</v>
       </c>
       <c r="M121" s="8" t="s">
-        <v>444</v>
+        <v>387</v>
       </c>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>11.06.2023</v>
+      </c>
+      <c r="K122" s="8">
+        <v>5</v>
+      </c>
+      <c r="L122" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="M122" s="8" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A123" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>11.06.2023</v>
+      </c>
+      <c r="K123" s="8">
+        <v>6</v>
+      </c>
+      <c r="L123" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="M123" s="8" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A124" s="8" t="str">
         <f>"05.08.2023"</f>
         <v>05.08.2023</v>
       </c>
-      <c r="B122" s="9" t="s">
+      <c r="B124" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C122" s="10" t="s">
+      <c r="C124" s="10" t="s">
         <v>454</v>
       </c>
-      <c r="D122" s="8" t="s">
+      <c r="D124" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="E122" s="8" t="s">
+      <c r="E124" s="8" t="s">
         <v>456</v>
       </c>
-      <c r="F122" s="8" t="s">
+      <c r="F124" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="G122" s="8" t="s">
+      <c r="G124" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="K122" s="8">
-        <v>1</v>
-      </c>
-      <c r="L122" s="8" t="s">
+      <c r="K124" s="8">
+        <v>1</v>
+      </c>
+      <c r="L124" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M122" s="8" t="s">
+      <c r="M124" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="N122" s="9" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A123" s="12" t="str">
+      <c r="N124" s="9" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A125" s="12" t="str">
         <f>"08.11.2023"</f>
         <v>08.11.2023</v>
       </c>
-      <c r="B123" s="9" t="s">
+      <c r="B125" s="9" t="s">
         <v>446</v>
       </c>
-      <c r="C123" s="10" t="s">
+      <c r="C125" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="D123" s="8" t="s">
+      <c r="D125" s="8" t="s">
         <v>448</v>
       </c>
-      <c r="E123" s="8" t="s">
+      <c r="E125" s="8" t="s">
         <v>449</v>
       </c>
-      <c r="F123" s="8" t="s">
+      <c r="F125" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="G123" s="8" t="s">
+      <c r="G125" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="K123" s="8">
-        <v>1</v>
-      </c>
-      <c r="L123" s="8" t="s">
+      <c r="K125" s="8">
+        <v>1</v>
+      </c>
+      <c r="L125" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="M123" s="8" t="s">
+      <c r="M125" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4998,9 +5057,9 @@
     <hyperlink ref="C51" r:id="rId2"/>
     <hyperlink ref="H109" r:id="rId3" display="https://urldefense.com/v3/__http:/www.youtube.com/@biostat_reviews__;!!N3hqHg43uw!qSFZ6CinavKXCScVyqzyOOZ1nqhhrcCXU560M_FxxlHb0YOvNuF3HkFI2dogiKDjjZmUQyYAPYejC--9qf1bJhfiDtG1Jng$"/>
     <hyperlink ref="C114" r:id="rId4"/>
-    <hyperlink ref="C123" r:id="rId5"/>
+    <hyperlink ref="C125" r:id="rId5"/>
     <hyperlink ref="C115" r:id="rId6"/>
-    <hyperlink ref="C122" r:id="rId7"/>
+    <hyperlink ref="C124" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>

</xml_diff>